<commit_message>
EPBDS-9610 fixing existing test table names in maven-plugin
</commit_message>
<xml_diff>
--- a/Util/openl-maven-plugin/it/openl-gen-datatypes/src/main/openl/rules/Datatype.xlsx
+++ b/Util/openl-maven-plugin/it/openl-gen-datatypes/src/main/openl/rules/Datatype.xlsx
@@ -1,32 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\Util\openl-maven-plugin\target\its\openl-gen-datatypes\src\main\openl\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\Util\openl-maven-plugin\it\openl-gen-datatypes\src\main\openl\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887EC8F5-E842-4C0C-A83B-0DEE67B70701}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="20700" windowHeight="11760"/>
+    <workbookView xWindow="-57720" yWindow="6450" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datatypes" sheetId="1" r:id="rId1"/>
     <sheet name="Methods" sheetId="2" r:id="rId2"/>
     <sheet name="Env" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Yury Molchan</author>
   </authors>
   <commentList>
-    <comment ref="D8" authorId="0" shapeId="0">
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -50,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="0" shapeId="0">
+    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -74,7 +85,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L8" authorId="0" shapeId="0">
+    <comment ref="L8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -98,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P8" authorId="0" shapeId="0">
+    <comment ref="P8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -122,7 +133,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D41" authorId="0" shapeId="0">
+    <comment ref="D41" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -146,7 +157,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H41" authorId="0" shapeId="0">
+    <comment ref="H41" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -170,7 +181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L41" authorId="0" shapeId="0">
+    <comment ref="L41" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -194,7 +205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P41" authorId="0" shapeId="0">
+    <comment ref="P41" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -218,7 +229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D57" authorId="0" shapeId="0">
+    <comment ref="D57" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -242,7 +253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H57" authorId="0" shapeId="0">
+    <comment ref="H57" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -266,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L57" authorId="0" shapeId="0">
+    <comment ref="L57" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -290,7 +301,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P57" authorId="0" shapeId="0">
+    <comment ref="P57" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -314,7 +325,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D90" authorId="0" shapeId="0">
+    <comment ref="D90" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -338,7 +349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H90" authorId="0" shapeId="0">
+    <comment ref="H90" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -362,7 +373,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L90" authorId="0" shapeId="0">
+    <comment ref="L90" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -386,7 +397,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P90" authorId="0" shapeId="0">
+    <comment ref="P90" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -410,7 +421,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D106" authorId="0" shapeId="0">
+    <comment ref="D106" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -434,7 +445,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H106" authorId="0" shapeId="0">
+    <comment ref="H106" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -458,7 +469,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L106" authorId="0" shapeId="0">
+    <comment ref="L106" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -482,7 +493,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P106" authorId="0" shapeId="0">
+    <comment ref="P106" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -506,7 +517,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D139" authorId="0" shapeId="0">
+    <comment ref="D139" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -530,7 +541,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H139" authorId="0" shapeId="0">
+    <comment ref="H139" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
       <text>
         <r>
           <rPr>
@@ -554,7 +565,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L139" authorId="0" shapeId="0">
+    <comment ref="L139" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
       <text>
         <r>
           <rPr>
@@ -578,7 +589,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P139" authorId="0" shapeId="0">
+    <comment ref="P139" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
       <text>
         <r>
           <rPr>
@@ -602,7 +613,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L152" authorId="0" shapeId="0">
+    <comment ref="L152" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
       <text>
         <r>
           <rPr>
@@ -1221,9 +1232,6 @@
     <t>result</t>
   </si>
   <si>
-    <t>Test evaluate evaluateTest()</t>
-  </si>
-  <si>
     <t>_res_.$equals$result</t>
   </si>
   <si>
@@ -1451,11 +1459,14 @@
   <si>
     <t>Test getBoxedWithModifiebleCollectionsCount boxedWithModifiebleCollectionsTest</t>
   </si>
+  <si>
+    <t>Test evaluate evaluateTest</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1696,17 +1707,41 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1736,33 +1771,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2103,32 +2114,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:R194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="J136" sqref="J136"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="7.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="27.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="52.28515625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="7.140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="16" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.68359375" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.68359375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.15625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.68359375" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="15.68359375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="7.15625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="27.68359375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.68359375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="52.26171875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="7.15625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="20.68359375" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="15.68359375" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13.578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F3" s="30" t="s">
         <v>181</v>
       </c>
@@ -2140,19 +2151,19 @@
       <c r="O3" s="30"/>
       <c r="P3" s="30"/>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F4" s="35" t="s">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F4" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="N4" s="35" t="s">
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="N4" s="40" t="s">
         <v>139</v>
       </c>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="30" t="s">
         <v>14</v>
       </c>
@@ -2163,18 +2174,18 @@
       </c>
       <c r="G7" s="30"/>
       <c r="H7" s="30"/>
-      <c r="J7" s="36" t="s">
+      <c r="J7" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
       <c r="N7" s="30" t="s">
         <v>137</v>
       </c>
       <c r="O7" s="30"/>
       <c r="P7" s="30"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="1" t="s">
         <v>192</v>
       </c>
@@ -2216,7 +2227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="17" t="s">
         <v>10</v>
       </c>
@@ -2255,7 +2266,7 @@
       </c>
       <c r="P9" s="17"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -2294,7 +2305,7 @@
       </c>
       <c r="P10" s="6"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="1" t="s">
         <v>0</v>
       </c>
@@ -2333,7 +2344,7 @@
       </c>
       <c r="P11" s="6"/>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
@@ -2372,7 +2383,7 @@
       </c>
       <c r="P12" s="6"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
@@ -2411,7 +2422,7 @@
       </c>
       <c r="P13" s="6"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="1" t="s">
         <v>8</v>
       </c>
@@ -2450,7 +2461,7 @@
       </c>
       <c r="P14" s="6"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
@@ -2489,7 +2500,7 @@
       </c>
       <c r="P15" s="6"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
@@ -2528,12 +2539,12 @@
       </c>
       <c r="P16" s="6"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>20</v>
@@ -2567,12 +2578,12 @@
       </c>
       <c r="P17" s="6"/>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>94</v>
@@ -2606,12 +2617,12 @@
       </c>
       <c r="P18" s="2"/>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D19" s="1">
         <v>7</v>
@@ -2645,12 +2656,12 @@
       </c>
       <c r="P19" s="6"/>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D20" s="1">
         <v>8</v>
@@ -2684,12 +2695,12 @@
       </c>
       <c r="P20" s="6"/>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="10" t="s">
         <v>144</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>2</v>
@@ -2720,12 +2731,12 @@
       </c>
       <c r="P21" s="10"/>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>2</v>
@@ -2756,12 +2767,12 @@
       </c>
       <c r="P22" s="6"/>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>2</v>
@@ -2792,12 +2803,12 @@
       </c>
       <c r="P23" s="6"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>2</v>
@@ -2828,12 +2839,12 @@
       </c>
       <c r="P24" s="6"/>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D25" s="21" t="s">
         <v>2</v>
@@ -2848,10 +2859,10 @@
       </c>
       <c r="H25" s="28"/>
       <c r="J25" s="21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K25" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L25" s="21"/>
       <c r="N25" s="22" t="str">
@@ -2864,12 +2875,12 @@
       </c>
       <c r="P25" s="21"/>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" s="21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D26" s="21" t="s">
         <v>2</v>
@@ -2884,10 +2895,10 @@
       </c>
       <c r="H26" s="28"/>
       <c r="J26" s="21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K26" s="21" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L26" s="21"/>
       <c r="N26" s="22" t="str">
@@ -2900,12 +2911,12 @@
       </c>
       <c r="P26" s="21"/>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" s="21" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D27" s="21" t="s">
         <v>2</v>
@@ -2920,10 +2931,10 @@
       </c>
       <c r="H27" s="28"/>
       <c r="J27" s="21" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K27" s="21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L27" s="21"/>
       <c r="N27" s="22" t="str">
@@ -2936,15 +2947,15 @@
       </c>
       <c r="P27" s="21"/>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="C28" s="22" t="s">
         <v>244</v>
       </c>
-      <c r="C28" s="22" t="s">
-        <v>245</v>
-      </c>
       <c r="D28" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F28" s="22" t="str">
         <f t="shared" si="5"/>
@@ -2959,10 +2970,10 @@
         <v>Male</v>
       </c>
       <c r="J28" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="K28" s="22" t="s">
         <v>244</v>
-      </c>
-      <c r="K28" s="22" t="s">
-        <v>245</v>
       </c>
       <c r="L28" s="22"/>
       <c r="N28" s="22" t="str">
@@ -2975,12 +2986,12 @@
       </c>
       <c r="P28" s="22"/>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D29" s="20" t="s">
         <v>2</v>
@@ -2995,10 +3006,10 @@
       </c>
       <c r="H29" s="28"/>
       <c r="J29" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K29" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L29" s="20"/>
       <c r="N29" s="22" t="str">
@@ -3011,7 +3022,7 @@
       </c>
       <c r="P29" s="20"/>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" s="20" t="s">
         <v>6</v>
       </c>
@@ -3047,12 +3058,12 @@
       </c>
       <c r="P30" s="20"/>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="C31" s="20" t="s">
         <v>211</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>212</v>
       </c>
       <c r="D31" s="20" t="s">
         <v>2</v>
@@ -3067,10 +3078,10 @@
       </c>
       <c r="H31" s="28"/>
       <c r="J31" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="K31" s="20" t="s">
         <v>211</v>
-      </c>
-      <c r="K31" s="20" t="s">
-        <v>212</v>
       </c>
       <c r="L31" s="20"/>
       <c r="N31" s="21" t="str">
@@ -3083,15 +3094,15 @@
       </c>
       <c r="P31" s="20"/>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="C32" s="24" t="s">
         <v>251</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="D32" s="24" t="s">
         <v>252</v>
-      </c>
-      <c r="D32" s="24" t="s">
-        <v>253</v>
       </c>
       <c r="F32" s="24" t="str">
         <f>"_res_." &amp; C32</f>
@@ -3106,10 +3117,10 @@
         <v>HALF_EVEN</v>
       </c>
       <c r="J32" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="K32" s="24" t="s">
         <v>251</v>
-      </c>
-      <c r="K32" s="24" t="s">
-        <v>252</v>
       </c>
       <c r="L32" s="24"/>
       <c r="N32" s="24" t="str">
@@ -3122,12 +3133,12 @@
       </c>
       <c r="P32" s="24"/>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" s="26" t="s">
         <v>192</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D33" s="26">
         <v>10.1</v>
@@ -3148,7 +3159,7 @@
         <v>192</v>
       </c>
       <c r="K33" s="26" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L33" s="26"/>
       <c r="N33" s="26" t="str">
@@ -3161,7 +3172,7 @@
       </c>
       <c r="P33" s="26"/>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F36" s="30" t="s">
         <v>180</v>
       </c>
@@ -3173,41 +3184,41 @@
       <c r="O36" s="30"/>
       <c r="P36" s="30"/>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F37" s="35" t="s">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F37" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="G37" s="35"/>
-      <c r="H37" s="35"/>
-      <c r="N37" s="35" t="s">
+      <c r="G37" s="40"/>
+      <c r="H37" s="40"/>
+      <c r="N37" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="O37" s="35"/>
-      <c r="P37" s="35"/>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O37" s="40"/>
+      <c r="P37" s="40"/>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" s="30" t="s">
         <v>88</v>
       </c>
       <c r="C40" s="30"/>
       <c r="D40" s="30"/>
-      <c r="F40" s="37" t="s">
+      <c r="F40" s="42" t="s">
         <v>162</v>
       </c>
-      <c r="G40" s="37"/>
-      <c r="H40" s="37"/>
-      <c r="J40" s="36" t="s">
+      <c r="G40" s="42"/>
+      <c r="H40" s="42"/>
+      <c r="J40" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="K40" s="36"/>
-      <c r="L40" s="36"/>
-      <c r="N40" s="37" t="s">
+      <c r="K40" s="41"/>
+      <c r="L40" s="41"/>
+      <c r="N40" s="42" t="s">
         <v>163</v>
       </c>
-      <c r="O40" s="37"/>
-      <c r="P40" s="37"/>
-    </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O40" s="42"/>
+      <c r="P40" s="42"/>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B41" s="17" t="s">
         <v>192</v>
       </c>
@@ -3249,7 +3260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B42" s="1" t="s">
         <v>39</v>
       </c>
@@ -3290,7 +3301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B43" s="1" t="s">
         <v>40</v>
       </c>
@@ -3331,7 +3342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B44" s="1" t="s">
         <v>41</v>
       </c>
@@ -3372,7 +3383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B45" s="1" t="s">
         <v>42</v>
       </c>
@@ -3413,7 +3424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B46" s="1" t="s">
         <v>43</v>
       </c>
@@ -3454,7 +3465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B47" s="1" t="s">
         <v>44</v>
       </c>
@@ -3495,7 +3506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B48" s="1" t="s">
         <v>46</v>
       </c>
@@ -3536,7 +3547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B49" s="1" t="s">
         <v>45</v>
       </c>
@@ -3575,7 +3586,7 @@
       </c>
       <c r="P49" s="6"/>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F52" s="30" t="s">
         <v>178</v>
       </c>
@@ -3587,19 +3598,19 @@
       <c r="O52" s="30"/>
       <c r="P52" s="30"/>
     </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F53" s="35" t="s">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F53" s="40" t="s">
         <v>156</v>
       </c>
-      <c r="G53" s="35"/>
-      <c r="H53" s="35"/>
-      <c r="N53" s="35" t="s">
+      <c r="G53" s="40"/>
+      <c r="H53" s="40"/>
+      <c r="N53" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="O53" s="35"/>
-      <c r="P53" s="35"/>
-    </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O53" s="40"/>
+      <c r="P53" s="40"/>
+    </row>
+    <row r="56" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B56" s="30" t="s">
         <v>142</v>
       </c>
@@ -3610,18 +3621,18 @@
       </c>
       <c r="G56" s="30"/>
       <c r="H56" s="30"/>
-      <c r="J56" s="36" t="s">
+      <c r="J56" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="K56" s="36"/>
-      <c r="L56" s="36"/>
+      <c r="K56" s="41"/>
+      <c r="L56" s="41"/>
       <c r="N56" s="30" t="s">
         <v>158</v>
       </c>
       <c r="O56" s="30"/>
       <c r="P56" s="30"/>
     </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B57" s="17" t="s">
         <v>192</v>
       </c>
@@ -3663,7 +3674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B58" s="1" t="s">
         <v>97</v>
       </c>
@@ -3702,7 +3713,7 @@
       </c>
       <c r="P58" s="12"/>
     </row>
-    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B59" s="1" t="s">
         <v>98</v>
       </c>
@@ -3741,7 +3752,7 @@
       </c>
       <c r="P59" s="12"/>
     </row>
-    <row r="60" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B60" s="1" t="s">
         <v>99</v>
       </c>
@@ -3780,7 +3791,7 @@
       </c>
       <c r="P60" s="12"/>
     </row>
-    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B61" s="1" t="s">
         <v>100</v>
       </c>
@@ -3819,7 +3830,7 @@
       </c>
       <c r="P61" s="12"/>
     </row>
-    <row r="62" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B62" s="1" t="s">
         <v>101</v>
       </c>
@@ -3858,7 +3869,7 @@
       </c>
       <c r="P62" s="12"/>
     </row>
-    <row r="63" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B63" s="1" t="s">
         <v>102</v>
       </c>
@@ -3897,7 +3908,7 @@
       </c>
       <c r="P63" s="12"/>
     </row>
-    <row r="64" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B64" s="1" t="s">
         <v>103</v>
       </c>
@@ -3936,7 +3947,7 @@
       </c>
       <c r="P64" s="12"/>
     </row>
-    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B65" s="1" t="s">
         <v>104</v>
       </c>
@@ -3975,7 +3986,7 @@
       </c>
       <c r="P65" s="12"/>
     </row>
-    <row r="66" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B66" s="1" t="s">
         <v>58</v>
       </c>
@@ -4014,7 +4025,7 @@
       </c>
       <c r="P66" s="12"/>
     </row>
-    <row r="67" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B67" s="1" t="s">
         <v>59</v>
       </c>
@@ -4053,7 +4064,7 @@
       </c>
       <c r="P67" s="2"/>
     </row>
-    <row r="68" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B68" s="1" t="s">
         <v>60</v>
       </c>
@@ -4092,7 +4103,7 @@
       </c>
       <c r="P68" s="12"/>
     </row>
-    <row r="69" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B69" s="1" t="s">
         <v>61</v>
       </c>
@@ -4131,7 +4142,7 @@
       </c>
       <c r="P69" s="12"/>
     </row>
-    <row r="70" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B70" s="10" t="s">
         <v>147</v>
       </c>
@@ -4167,9 +4178,9 @@
       </c>
       <c r="P70" s="12"/>
     </row>
-    <row r="71" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B71" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>35</v>
@@ -4203,7 +4214,7 @@
       </c>
       <c r="P71" s="12"/>
     </row>
-    <row r="72" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B72" s="1" t="s">
         <v>115</v>
       </c>
@@ -4239,7 +4250,7 @@
       </c>
       <c r="P72" s="12"/>
     </row>
-    <row r="73" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B73" s="1" t="s">
         <v>116</v>
       </c>
@@ -4275,12 +4286,12 @@
       </c>
       <c r="P73" s="12"/>
     </row>
-    <row r="74" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B74" s="21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C74" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D74" s="21" t="s">
         <v>2</v>
@@ -4295,10 +4306,10 @@
       </c>
       <c r="H74" s="28"/>
       <c r="J74" s="21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K74" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L74" s="21"/>
       <c r="N74" s="21" t="str">
@@ -4311,12 +4322,12 @@
       </c>
       <c r="P74" s="21"/>
     </row>
-    <row r="75" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B75" s="21" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C75" s="21" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D75" s="21" t="s">
         <v>2</v>
@@ -4331,10 +4342,10 @@
       </c>
       <c r="H75" s="28"/>
       <c r="J75" s="21" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K75" s="21" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L75" s="21"/>
       <c r="N75" s="21" t="str">
@@ -4347,12 +4358,12 @@
       </c>
       <c r="P75" s="21"/>
     </row>
-    <row r="76" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B76" s="21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C76" s="21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D76" s="21" t="s">
         <v>2</v>
@@ -4367,10 +4378,10 @@
       </c>
       <c r="H76" s="28"/>
       <c r="J76" s="21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K76" s="21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L76" s="21"/>
       <c r="N76" s="22" t="str">
@@ -4383,15 +4394,15 @@
       </c>
       <c r="P76" s="21"/>
     </row>
-    <row r="77" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B77" s="22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C77" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D77" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F77" s="22" t="str">
         <f t="shared" si="11"/>
@@ -4406,10 +4417,10 @@
         <v>Male, Female</v>
       </c>
       <c r="J77" s="22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K77" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L77" s="22"/>
       <c r="N77" s="22" t="str">
@@ -4422,12 +4433,12 @@
       </c>
       <c r="P77" s="22"/>
     </row>
-    <row r="78" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B78" s="20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C78" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D78" s="20" t="s">
         <v>2</v>
@@ -4442,10 +4453,10 @@
       </c>
       <c r="H78" s="28"/>
       <c r="J78" s="20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K78" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L78" s="20"/>
       <c r="N78" s="22" t="str">
@@ -4458,9 +4469,9 @@
       </c>
       <c r="P78" s="20"/>
     </row>
-    <row r="79" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B79" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C79" s="20" t="s">
         <v>7</v>
@@ -4478,7 +4489,7 @@
       </c>
       <c r="H79" s="28"/>
       <c r="J79" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K79" s="20" t="s">
         <v>7</v>
@@ -4494,12 +4505,12 @@
       </c>
       <c r="P79" s="20"/>
     </row>
-    <row r="80" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B80" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C80" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D80" s="20" t="s">
         <v>2</v>
@@ -4514,10 +4525,10 @@
       </c>
       <c r="H80" s="28"/>
       <c r="J80" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K80" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L80" s="20"/>
       <c r="N80" s="21" t="str">
@@ -4530,15 +4541,15 @@
       </c>
       <c r="P80" s="20"/>
     </row>
-    <row r="81" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B81" s="25" t="s">
+        <v>253</v>
+      </c>
+      <c r="C81" s="25" t="s">
+        <v>251</v>
+      </c>
+      <c r="D81" s="25" t="s">
         <v>254</v>
-      </c>
-      <c r="C81" s="25" t="s">
-        <v>252</v>
-      </c>
-      <c r="D81" s="25" t="s">
-        <v>255</v>
       </c>
       <c r="F81" s="25" t="str">
         <f>"_res_." &amp; C81</f>
@@ -4553,10 +4564,10 @@
         <v>UP, DOWN</v>
       </c>
       <c r="J81" s="25" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K81" s="25" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="L81" s="25"/>
       <c r="N81" s="25" t="str">
@@ -4569,15 +4580,15 @@
       </c>
       <c r="P81" s="25"/>
     </row>
-    <row r="82" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B82" s="26" t="s">
+        <v>257</v>
+      </c>
+      <c r="C82" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="D82" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="C82" s="26" t="s">
-        <v>257</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>259</v>
       </c>
       <c r="F82" s="26" t="str">
         <f>"_res_." &amp; C82</f>
@@ -4592,10 +4603,10 @@
         <v>10.1, 22.4</v>
       </c>
       <c r="J82" s="26" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K82" s="26" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L82" s="26"/>
       <c r="N82" s="26" t="str">
@@ -4608,7 +4619,7 @@
       </c>
       <c r="P82" s="26"/>
     </row>
-    <row r="85" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F85" s="30" t="s">
         <v>176</v>
       </c>
@@ -4620,41 +4631,41 @@
       <c r="O85" s="30"/>
       <c r="P85" s="30"/>
     </row>
-    <row r="86" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F86" s="35" t="s">
+    <row r="86" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F86" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="G86" s="35"/>
-      <c r="H86" s="35"/>
-      <c r="N86" s="35" t="s">
+      <c r="G86" s="40"/>
+      <c r="H86" s="40"/>
+      <c r="N86" s="40" t="s">
         <v>161</v>
       </c>
-      <c r="O86" s="35"/>
-      <c r="P86" s="35"/>
-    </row>
-    <row r="89" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B89" s="34" t="s">
+      <c r="O86" s="40"/>
+      <c r="P86" s="40"/>
+    </row>
+    <row r="89" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B89" s="43" t="s">
         <v>143</v>
       </c>
-      <c r="C89" s="34"/>
-      <c r="D89" s="34"/>
+      <c r="C89" s="43"/>
+      <c r="D89" s="43"/>
       <c r="F89" s="30" t="s">
         <v>160</v>
       </c>
       <c r="G89" s="30"/>
       <c r="H89" s="30"/>
-      <c r="J89" s="36" t="s">
+      <c r="J89" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="K89" s="36"/>
-      <c r="L89" s="36"/>
-      <c r="N89" s="37" t="s">
+      <c r="K89" s="41"/>
+      <c r="L89" s="41"/>
+      <c r="N89" s="42" t="s">
         <v>164</v>
       </c>
-      <c r="O89" s="37"/>
-      <c r="P89" s="37"/>
-    </row>
-    <row r="90" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O89" s="42"/>
+      <c r="P89" s="42"/>
+    </row>
+    <row r="90" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B90" s="17" t="s">
         <v>192</v>
       </c>
@@ -4696,7 +4707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B91" s="1" t="s">
         <v>47</v>
       </c>
@@ -4734,7 +4745,7 @@
       </c>
       <c r="P91" s="13"/>
     </row>
-    <row r="92" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B92" s="1" t="s">
         <v>48</v>
       </c>
@@ -4772,7 +4783,7 @@
       </c>
       <c r="P92" s="13"/>
     </row>
-    <row r="93" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B93" s="1" t="s">
         <v>49</v>
       </c>
@@ -4810,7 +4821,7 @@
       </c>
       <c r="P93" s="13"/>
     </row>
-    <row r="94" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B94" s="1" t="s">
         <v>50</v>
       </c>
@@ -4848,7 +4859,7 @@
       </c>
       <c r="P94" s="13"/>
     </row>
-    <row r="95" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B95" s="1" t="s">
         <v>51</v>
       </c>
@@ -4886,7 +4897,7 @@
       </c>
       <c r="P95" s="13"/>
     </row>
-    <row r="96" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B96" s="1" t="s">
         <v>52</v>
       </c>
@@ -4924,7 +4935,7 @@
       </c>
       <c r="P96" s="13"/>
     </row>
-    <row r="97" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B97" s="1" t="s">
         <v>53</v>
       </c>
@@ -4962,7 +4973,7 @@
       </c>
       <c r="P97" s="13"/>
     </row>
-    <row r="98" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B98" s="1" t="s">
         <v>54</v>
       </c>
@@ -5000,7 +5011,7 @@
       </c>
       <c r="P98" s="13"/>
     </row>
-    <row r="101" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F101" s="30" t="s">
         <v>167</v>
       </c>
@@ -5012,41 +5023,41 @@
       <c r="O101" s="30"/>
       <c r="P101" s="30"/>
     </row>
-    <row r="102" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F102" s="35" t="s">
+    <row r="102" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F102" s="40" t="s">
         <v>168</v>
       </c>
-      <c r="G102" s="35"/>
-      <c r="H102" s="35"/>
-      <c r="N102" s="35" t="s">
+      <c r="G102" s="40"/>
+      <c r="H102" s="40"/>
+      <c r="N102" s="40" t="s">
         <v>165</v>
       </c>
-      <c r="O102" s="35"/>
-      <c r="P102" s="35"/>
-    </row>
-    <row r="105" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B105" s="34" t="s">
+      <c r="O102" s="40"/>
+      <c r="P102" s="40"/>
+    </row>
+    <row r="105" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B105" s="43" t="s">
         <v>154</v>
       </c>
-      <c r="C105" s="34"/>
-      <c r="D105" s="34"/>
+      <c r="C105" s="43"/>
+      <c r="D105" s="43"/>
       <c r="F105" s="30" t="s">
         <v>190</v>
       </c>
       <c r="G105" s="30"/>
       <c r="H105" s="30"/>
-      <c r="J105" s="36" t="s">
+      <c r="J105" s="41" t="s">
         <v>153</v>
       </c>
-      <c r="K105" s="36"/>
-      <c r="L105" s="36"/>
+      <c r="K105" s="41"/>
+      <c r="L105" s="41"/>
       <c r="N105" s="30" t="s">
         <v>191</v>
       </c>
       <c r="O105" s="30"/>
       <c r="P105" s="30"/>
     </row>
-    <row r="106" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B106" s="17" t="s">
         <v>192</v>
       </c>
@@ -5088,7 +5099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B107" s="1" t="s">
         <v>105</v>
       </c>
@@ -5124,7 +5135,7 @@
       </c>
       <c r="P107" s="13"/>
     </row>
-    <row r="108" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B108" s="1" t="s">
         <v>106</v>
       </c>
@@ -5160,7 +5171,7 @@
       </c>
       <c r="P108" s="13"/>
     </row>
-    <row r="109" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B109" s="1" t="s">
         <v>107</v>
       </c>
@@ -5196,7 +5207,7 @@
       </c>
       <c r="P109" s="13"/>
     </row>
-    <row r="110" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B110" s="1" t="s">
         <v>108</v>
       </c>
@@ -5232,7 +5243,7 @@
       </c>
       <c r="P110" s="13"/>
     </row>
-    <row r="111" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B111" s="1" t="s">
         <v>109</v>
       </c>
@@ -5268,7 +5279,7 @@
       </c>
       <c r="P111" s="13"/>
     </row>
-    <row r="112" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B112" s="1" t="s">
         <v>110</v>
       </c>
@@ -5304,7 +5315,7 @@
       </c>
       <c r="P112" s="13"/>
     </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B113" s="1" t="s">
         <v>111</v>
       </c>
@@ -5340,7 +5351,7 @@
       </c>
       <c r="P113" s="13"/>
     </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B114" s="1" t="s">
         <v>112</v>
       </c>
@@ -5376,7 +5387,7 @@
       </c>
       <c r="P114" s="13"/>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B115" s="1" t="s">
         <v>71</v>
       </c>
@@ -5412,7 +5423,7 @@
       </c>
       <c r="P115" s="13"/>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B116" s="1" t="s">
         <v>72</v>
       </c>
@@ -5448,7 +5459,7 @@
       </c>
       <c r="P116" s="2"/>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B117" s="1" t="s">
         <v>73</v>
       </c>
@@ -5484,7 +5495,7 @@
       </c>
       <c r="P117" s="13"/>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B118" s="1" t="s">
         <v>74</v>
       </c>
@@ -5520,7 +5531,7 @@
       </c>
       <c r="P118" s="13"/>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B119" s="10" t="s">
         <v>146</v>
       </c>
@@ -5556,7 +5567,7 @@
       </c>
       <c r="P119" s="13"/>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B120" s="1" t="s">
         <v>117</v>
       </c>
@@ -5592,7 +5603,7 @@
       </c>
       <c r="P120" s="13"/>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B121" s="1" t="s">
         <v>118</v>
       </c>
@@ -5628,7 +5639,7 @@
       </c>
       <c r="P121" s="13"/>
     </row>
-    <row r="122" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B122" s="1" t="s">
         <v>119</v>
       </c>
@@ -5664,12 +5675,12 @@
       </c>
       <c r="P122" s="13"/>
     </row>
-    <row r="123" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B123" s="21" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C123" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D123" s="21" t="s">
         <v>2</v>
@@ -5684,10 +5695,10 @@
       </c>
       <c r="H123" s="21"/>
       <c r="J123" s="21" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K123" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L123" s="21"/>
       <c r="N123" s="21" t="str">
@@ -5700,12 +5711,12 @@
       </c>
       <c r="P123" s="21"/>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B124" s="21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C124" s="21" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D124" s="21" t="s">
         <v>2</v>
@@ -5720,10 +5731,10 @@
       </c>
       <c r="H124" s="21"/>
       <c r="J124" s="21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K124" s="21" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L124" s="21"/>
       <c r="N124" s="21" t="str">
@@ -5736,12 +5747,12 @@
       </c>
       <c r="P124" s="21"/>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B125" s="21" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C125" s="21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D125" s="21" t="s">
         <v>2</v>
@@ -5756,10 +5767,10 @@
       </c>
       <c r="H125" s="21"/>
       <c r="J125" s="21" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K125" s="21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L125" s="21"/>
       <c r="N125" s="21" t="str">
@@ -5772,12 +5783,12 @@
       </c>
       <c r="P125" s="21"/>
     </row>
-    <row r="126" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B126" s="22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C126" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D126" s="22" t="s">
         <v>2</v>
@@ -5792,10 +5803,10 @@
       </c>
       <c r="H126" s="22"/>
       <c r="J126" s="22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K126" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L126" s="22"/>
       <c r="N126" s="22" t="str">
@@ -5808,12 +5819,12 @@
       </c>
       <c r="P126" s="22"/>
     </row>
-    <row r="127" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B127" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="C127" s="20" t="s">
         <v>238</v>
-      </c>
-      <c r="C127" s="20" t="s">
-        <v>239</v>
       </c>
       <c r="D127" s="20" t="s">
         <v>2</v>
@@ -5828,10 +5839,10 @@
       </c>
       <c r="H127" s="20"/>
       <c r="J127" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="K127" s="20" t="s">
         <v>238</v>
-      </c>
-      <c r="K127" s="20" t="s">
-        <v>239</v>
       </c>
       <c r="L127" s="20"/>
       <c r="N127" s="21" t="str">
@@ -5844,9 +5855,9 @@
       </c>
       <c r="P127" s="20"/>
     </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B128" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C128" s="20" t="s">
         <v>7</v>
@@ -5864,7 +5875,7 @@
       </c>
       <c r="H128" s="20"/>
       <c r="J128" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K128" s="20" t="s">
         <v>7</v>
@@ -5880,12 +5891,12 @@
       </c>
       <c r="P128" s="20"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B129" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C129" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D129" s="20" t="s">
         <v>2</v>
@@ -5900,10 +5911,10 @@
       </c>
       <c r="H129" s="20"/>
       <c r="J129" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K129" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L129" s="20"/>
       <c r="N129" s="21" t="str">
@@ -5916,12 +5927,12 @@
       </c>
       <c r="P129" s="20"/>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B130" s="25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C130" s="25" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D130" s="25" t="s">
         <v>2</v>
@@ -5936,10 +5947,10 @@
       </c>
       <c r="H130" s="25"/>
       <c r="J130" s="25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K130" s="25" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="L130" s="25"/>
       <c r="N130" s="25" t="str">
@@ -5952,12 +5963,12 @@
       </c>
       <c r="P130" s="25"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B131" s="26" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C131" s="26" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D131" s="26" t="s">
         <v>2</v>
@@ -5972,10 +5983,10 @@
       </c>
       <c r="H131" s="2"/>
       <c r="J131" s="26" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K131" s="26" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L131" s="26"/>
       <c r="N131" s="26" t="str">
@@ -5988,7 +5999,7 @@
       </c>
       <c r="P131" s="26"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F134" s="30" t="s">
         <v>174</v>
       </c>
@@ -6000,41 +6011,41 @@
       <c r="O134" s="30"/>
       <c r="P134" s="30"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F135" s="35" t="s">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F135" s="40" t="s">
         <v>169</v>
       </c>
-      <c r="G135" s="35"/>
-      <c r="H135" s="35"/>
-      <c r="N135" s="35" t="s">
+      <c r="G135" s="40"/>
+      <c r="H135" s="40"/>
+      <c r="N135" s="40" t="s">
         <v>171</v>
       </c>
-      <c r="O135" s="35"/>
-      <c r="P135" s="35"/>
-    </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B138" s="34" t="s">
+      <c r="O135" s="40"/>
+      <c r="P135" s="40"/>
+    </row>
+    <row r="138" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B138" s="43" t="s">
         <v>151</v>
       </c>
-      <c r="C138" s="34"/>
-      <c r="D138" s="34"/>
-      <c r="F138" s="37" t="s">
+      <c r="C138" s="43"/>
+      <c r="D138" s="43"/>
+      <c r="F138" s="42" t="s">
         <v>170</v>
       </c>
-      <c r="G138" s="37"/>
-      <c r="H138" s="37"/>
-      <c r="J138" s="36" t="s">
+      <c r="G138" s="42"/>
+      <c r="H138" s="42"/>
+      <c r="J138" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="K138" s="36"/>
-      <c r="L138" s="36"/>
-      <c r="N138" s="37" t="s">
+      <c r="K138" s="41"/>
+      <c r="L138" s="41"/>
+      <c r="N138" s="42" t="s">
         <v>172</v>
       </c>
-      <c r="O138" s="37"/>
-      <c r="P138" s="37"/>
-    </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O138" s="42"/>
+      <c r="P138" s="42"/>
+    </row>
+    <row r="139" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B139" s="17" t="s">
         <v>192</v>
       </c>
@@ -6076,7 +6087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B140" s="1" t="s">
         <v>63</v>
       </c>
@@ -6112,7 +6123,7 @@
       </c>
       <c r="P140" s="13"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B141" s="1" t="s">
         <v>64</v>
       </c>
@@ -6148,7 +6159,7 @@
       </c>
       <c r="P141" s="13"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B142" s="1" t="s">
         <v>65</v>
       </c>
@@ -6184,7 +6195,7 @@
       </c>
       <c r="P142" s="13"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B143" s="1" t="s">
         <v>66</v>
       </c>
@@ -6220,7 +6231,7 @@
       </c>
       <c r="P143" s="13"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B144" s="1" t="s">
         <v>67</v>
       </c>
@@ -6256,7 +6267,7 @@
       </c>
       <c r="P144" s="13"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B145" s="1" t="s">
         <v>68</v>
       </c>
@@ -6292,7 +6303,7 @@
       </c>
       <c r="P145" s="13"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B146" s="1" t="s">
         <v>69</v>
       </c>
@@ -6328,7 +6339,7 @@
       </c>
       <c r="P146" s="13"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B147" s="1" t="s">
         <v>70</v>
       </c>
@@ -6364,143 +6375,143 @@
       </c>
       <c r="P147" s="13"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B151" s="30" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C151" s="30"/>
       <c r="D151" s="30"/>
       <c r="F151" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G151" s="30"/>
       <c r="H151" s="30"/>
       <c r="J151" s="30" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K151" s="30"/>
       <c r="L151" s="30"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B152" s="31" t="s">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B152" s="55" t="s">
+        <v>240</v>
+      </c>
+      <c r="C152" s="56"/>
+      <c r="D152" s="57"/>
+      <c r="F152" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="G152" s="32"/>
+      <c r="H152" s="33"/>
+      <c r="J152" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="K152" s="29" t="s">
+        <v>264</v>
+      </c>
+      <c r="L152" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="153" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B153" s="55" t="s">
         <v>241</v>
       </c>
-      <c r="C152" s="32"/>
-      <c r="D152" s="33"/>
-      <c r="F152" s="49" t="s">
-        <v>262</v>
-      </c>
-      <c r="G152" s="50"/>
-      <c r="H152" s="51"/>
-      <c r="J152" s="29" t="s">
-        <v>264</v>
-      </c>
-      <c r="K152" s="29" t="s">
-        <v>265</v>
-      </c>
-      <c r="L152" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B153" s="31" t="s">
+      <c r="C153" s="56"/>
+      <c r="D153" s="57"/>
+      <c r="F153" s="34"/>
+      <c r="G153" s="35"/>
+      <c r="H153" s="36"/>
+    </row>
+    <row r="154" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B154" s="55" t="s">
         <v>242</v>
       </c>
-      <c r="C153" s="32"/>
-      <c r="D153" s="33"/>
-      <c r="F153" s="52"/>
-      <c r="G153" s="53"/>
-      <c r="H153" s="54"/>
-    </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B154" s="31" t="s">
-        <v>243</v>
-      </c>
-      <c r="C154" s="32"/>
-      <c r="D154" s="33"/>
-      <c r="F154" s="52"/>
-      <c r="G154" s="53"/>
-      <c r="H154" s="54"/>
-    </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F155" s="52"/>
-      <c r="G155" s="53"/>
-      <c r="H155" s="54"/>
-    </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F156" s="52"/>
-      <c r="G156" s="53"/>
-      <c r="H156" s="54"/>
-    </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C154" s="56"/>
+      <c r="D154" s="57"/>
+      <c r="F154" s="34"/>
+      <c r="G154" s="35"/>
+      <c r="H154" s="36"/>
+    </row>
+    <row r="155" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F155" s="34"/>
+      <c r="G155" s="35"/>
+      <c r="H155" s="36"/>
+    </row>
+    <row r="156" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F156" s="34"/>
+      <c r="G156" s="35"/>
+      <c r="H156" s="36"/>
+    </row>
+    <row r="157" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B157" s="30" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C157" s="30"/>
       <c r="D157" s="30"/>
-      <c r="F157" s="52"/>
-      <c r="G157" s="53"/>
-      <c r="H157" s="54"/>
-    </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="F157" s="34"/>
+      <c r="G157" s="35"/>
+      <c r="H157" s="36"/>
+    </row>
+    <row r="158" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B158" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C158" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C158" s="1" t="s">
-        <v>245</v>
-      </c>
       <c r="D158" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="F158" s="52"/>
-      <c r="G158" s="53"/>
-      <c r="H158" s="54"/>
-    </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+      <c r="F158" s="34"/>
+      <c r="G158" s="35"/>
+      <c r="H158" s="36"/>
+    </row>
+    <row r="159" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B159" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D159" s="1"/>
-      <c r="F159" s="52"/>
-      <c r="G159" s="53"/>
-      <c r="H159" s="54"/>
-    </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="F159" s="34"/>
+      <c r="G159" s="35"/>
+      <c r="H159" s="36"/>
+    </row>
+    <row r="160" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B160" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D160" s="1"/>
-      <c r="F160" s="52"/>
-      <c r="G160" s="53"/>
-      <c r="H160" s="54"/>
-    </row>
-    <row r="161" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F161" s="52"/>
-      <c r="G161" s="53"/>
-      <c r="H161" s="54"/>
-    </row>
-    <row r="162" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F162" s="52"/>
-      <c r="G162" s="53"/>
-      <c r="H162" s="54"/>
-    </row>
-    <row r="163" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F160" s="34"/>
+      <c r="G160" s="35"/>
+      <c r="H160" s="36"/>
+    </row>
+    <row r="161" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="F161" s="34"/>
+      <c r="G161" s="35"/>
+      <c r="H161" s="36"/>
+    </row>
+    <row r="162" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="F162" s="34"/>
+      <c r="G162" s="35"/>
+      <c r="H162" s="36"/>
+    </row>
+    <row r="163" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B163" s="30" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C163" s="30"/>
       <c r="D163" s="30"/>
-      <c r="F163" s="55"/>
-      <c r="G163" s="56"/>
-      <c r="H163" s="57"/>
-    </row>
-    <row r="164" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F163" s="37"/>
+      <c r="G163" s="38"/>
+      <c r="H163" s="39"/>
+    </row>
+    <row r="164" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B164" s="23" t="s">
         <v>0</v>
       </c>
@@ -6511,7 +6522,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="165" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B165" s="1" t="s">
         <v>4</v>
       </c>
@@ -6520,7 +6531,7 @@
       </c>
       <c r="D165" s="1"/>
     </row>
-    <row r="166" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B166" s="1" t="s">
         <v>6</v>
       </c>
@@ -6531,14 +6542,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B169" s="30" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C169" s="30"/>
       <c r="D169" s="30"/>
     </row>
-    <row r="170" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B170" s="1" t="s">
         <v>8</v>
       </c>
@@ -6549,18 +6560,18 @@
         <v>150</v>
       </c>
     </row>
-    <row r="171" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B171" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C171" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="C171" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="D171" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B172" s="1" t="s">
         <v>6</v>
       </c>
@@ -6569,211 +6580,261 @@
       </c>
       <c r="D172" s="1"/>
     </row>
-    <row r="175" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B175" s="36" t="s">
-        <v>249</v>
-      </c>
-      <c r="C175" s="36"/>
-      <c r="D175" s="36"/>
-      <c r="E175" s="36"/>
-      <c r="F175" s="36"/>
-    </row>
-    <row r="176" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B175" s="41" t="s">
+        <v>248</v>
+      </c>
+      <c r="C175" s="41"/>
+      <c r="D175" s="41"/>
+      <c r="E175" s="41"/>
+      <c r="F175" s="41"/>
+    </row>
+    <row r="176" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B176" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C176" s="43" t="s">
+      <c r="C176" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="D176" s="44"/>
-      <c r="E176" s="44"/>
-      <c r="F176" s="45"/>
-    </row>
-    <row r="177" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D176" s="50"/>
+      <c r="E176" s="50"/>
+      <c r="F176" s="51"/>
+    </row>
+    <row r="177" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B177" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C177" s="46" t="s">
+      <c r="C177" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="D177" s="47"/>
-      <c r="E177" s="47"/>
-      <c r="F177" s="48"/>
-    </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D177" s="53"/>
+      <c r="E177" s="53"/>
+      <c r="F177" s="54"/>
+    </row>
+    <row r="178" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B178" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C178" s="42" t="s">
+      <c r="C178" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="D178" s="39"/>
-      <c r="E178" s="39"/>
-      <c r="F178" s="40"/>
-    </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D178" s="45"/>
+      <c r="E178" s="45"/>
+      <c r="F178" s="46"/>
+    </row>
+    <row r="179" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B179" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C179" s="41" t="s">
+      <c r="C179" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="D179" s="41"/>
-      <c r="E179" s="41"/>
-      <c r="F179" s="41"/>
-    </row>
-    <row r="180" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D179" s="47"/>
+      <c r="E179" s="47"/>
+      <c r="F179" s="47"/>
+    </row>
+    <row r="180" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B180" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C180" s="38" t="s">
-        <v>250</v>
-      </c>
-      <c r="D180" s="39"/>
-      <c r="E180" s="39"/>
-      <c r="F180" s="40"/>
-    </row>
-    <row r="182" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C180" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="D180" s="45"/>
+      <c r="E180" s="45"/>
+      <c r="F180" s="46"/>
+    </row>
+    <row r="182" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B182" s="30" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C182" s="30"/>
       <c r="D182" s="30"/>
     </row>
-    <row r="183" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B183" s="49" t="s">
-        <v>263</v>
-      </c>
-      <c r="C183" s="50" t="s">
+    <row r="183" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B183" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="D183" s="51" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="184" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B184" s="52" t="s">
-        <v>262</v>
-      </c>
-      <c r="C184" s="53" t="s">
-        <v>262</v>
-      </c>
-      <c r="D184" s="54" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="185" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B185" s="52" t="s">
-        <v>262</v>
-      </c>
-      <c r="C185" s="53" t="s">
-        <v>262</v>
-      </c>
-      <c r="D185" s="54" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="186" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B186" s="52" t="s">
-        <v>262</v>
-      </c>
-      <c r="C186" s="53" t="s">
-        <v>262</v>
-      </c>
-      <c r="D186" s="54" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="187" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B187" s="52" t="s">
-        <v>262</v>
-      </c>
-      <c r="C187" s="53" t="s">
-        <v>262</v>
-      </c>
-      <c r="D187" s="54" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="188" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B188" s="52" t="s">
-        <v>262</v>
-      </c>
-      <c r="C188" s="53" t="s">
-        <v>262</v>
-      </c>
-      <c r="D188" s="54" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="189" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B189" s="52" t="s">
-        <v>262</v>
-      </c>
-      <c r="C189" s="53" t="s">
-        <v>262</v>
-      </c>
-      <c r="D189" s="54" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="190" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B190" s="52" t="s">
-        <v>262</v>
-      </c>
-      <c r="C190" s="53" t="s">
-        <v>262</v>
-      </c>
-      <c r="D190" s="54" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="191" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B191" s="52" t="s">
-        <v>262</v>
-      </c>
-      <c r="C191" s="53" t="s">
-        <v>262</v>
-      </c>
-      <c r="D191" s="54" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="192" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B192" s="52" t="s">
-        <v>262</v>
-      </c>
-      <c r="C192" s="53" t="s">
-        <v>262</v>
-      </c>
-      <c r="D192" s="54" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B193" s="52" t="s">
-        <v>262</v>
-      </c>
-      <c r="C193" s="53" t="s">
-        <v>262</v>
-      </c>
-      <c r="D193" s="54" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B194" s="55" t="s">
-        <v>262</v>
-      </c>
-      <c r="C194" s="56" t="s">
-        <v>262</v>
-      </c>
-      <c r="D194" s="57" t="s">
-        <v>262</v>
+      <c r="C183" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="D183" s="33" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="184" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B184" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="C184" s="35" t="s">
+        <v>261</v>
+      </c>
+      <c r="D184" s="36" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="185" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B185" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="C185" s="35" t="s">
+        <v>261</v>
+      </c>
+      <c r="D185" s="36" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="186" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B186" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="C186" s="35" t="s">
+        <v>261</v>
+      </c>
+      <c r="D186" s="36" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="187" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B187" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="C187" s="35" t="s">
+        <v>261</v>
+      </c>
+      <c r="D187" s="36" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="188" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B188" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="C188" s="35" t="s">
+        <v>261</v>
+      </c>
+      <c r="D188" s="36" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="189" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B189" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="C189" s="35" t="s">
+        <v>261</v>
+      </c>
+      <c r="D189" s="36" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="190" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B190" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="C190" s="35" t="s">
+        <v>261</v>
+      </c>
+      <c r="D190" s="36" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="191" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B191" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="C191" s="35" t="s">
+        <v>261</v>
+      </c>
+      <c r="D191" s="36" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="192" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B192" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="C192" s="35" t="s">
+        <v>261</v>
+      </c>
+      <c r="D192" s="36" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="193" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B193" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="C193" s="35" t="s">
+        <v>261</v>
+      </c>
+      <c r="D193" s="36" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B194" s="37" t="s">
+        <v>261</v>
+      </c>
+      <c r="C194" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="D194" s="39" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="66">
+    <mergeCell ref="B151:D151"/>
+    <mergeCell ref="B152:D152"/>
+    <mergeCell ref="B153:D153"/>
+    <mergeCell ref="B154:D154"/>
+    <mergeCell ref="F105:H105"/>
+    <mergeCell ref="B138:D138"/>
+    <mergeCell ref="B105:D105"/>
+    <mergeCell ref="F151:H151"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="N36:P36"/>
+    <mergeCell ref="N37:P37"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="N52:P52"/>
+    <mergeCell ref="N53:P53"/>
+    <mergeCell ref="N56:P56"/>
+    <mergeCell ref="F85:H85"/>
+    <mergeCell ref="N85:P85"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="C180:F180"/>
+    <mergeCell ref="C179:F179"/>
+    <mergeCell ref="B175:F175"/>
+    <mergeCell ref="B157:D157"/>
+    <mergeCell ref="B163:D163"/>
+    <mergeCell ref="C178:F178"/>
+    <mergeCell ref="C176:F176"/>
+    <mergeCell ref="C177:F177"/>
+    <mergeCell ref="B169:D169"/>
+    <mergeCell ref="B89:D89"/>
+    <mergeCell ref="F89:H89"/>
+    <mergeCell ref="N89:P89"/>
+    <mergeCell ref="N40:P40"/>
+    <mergeCell ref="F86:H86"/>
+    <mergeCell ref="J138:L138"/>
+    <mergeCell ref="N86:P86"/>
+    <mergeCell ref="J89:L89"/>
+    <mergeCell ref="J56:L56"/>
+    <mergeCell ref="J40:L40"/>
     <mergeCell ref="B182:D182"/>
     <mergeCell ref="B183:D194"/>
     <mergeCell ref="J151:L151"/>
@@ -6790,56 +6851,6 @@
     <mergeCell ref="F134:H134"/>
     <mergeCell ref="F135:H135"/>
     <mergeCell ref="F138:H138"/>
-    <mergeCell ref="J138:L138"/>
-    <mergeCell ref="N86:P86"/>
-    <mergeCell ref="J89:L89"/>
-    <mergeCell ref="J56:L56"/>
-    <mergeCell ref="J40:L40"/>
-    <mergeCell ref="B89:D89"/>
-    <mergeCell ref="F89:H89"/>
-    <mergeCell ref="N89:P89"/>
-    <mergeCell ref="N40:P40"/>
-    <mergeCell ref="F86:H86"/>
-    <mergeCell ref="C180:F180"/>
-    <mergeCell ref="C179:F179"/>
-    <mergeCell ref="B175:F175"/>
-    <mergeCell ref="B157:D157"/>
-    <mergeCell ref="B163:D163"/>
-    <mergeCell ref="C178:F178"/>
-    <mergeCell ref="C176:F176"/>
-    <mergeCell ref="C177:F177"/>
-    <mergeCell ref="B169:D169"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="N52:P52"/>
-    <mergeCell ref="N53:P53"/>
-    <mergeCell ref="N56:P56"/>
-    <mergeCell ref="F85:H85"/>
-    <mergeCell ref="N85:P85"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="N36:P36"/>
-    <mergeCell ref="N37:P37"/>
-    <mergeCell ref="B151:D151"/>
-    <mergeCell ref="B152:D152"/>
-    <mergeCell ref="B153:D153"/>
-    <mergeCell ref="B154:D154"/>
-    <mergeCell ref="F105:H105"/>
-    <mergeCell ref="B138:D138"/>
-    <mergeCell ref="B105:D105"/>
-    <mergeCell ref="F151:H151"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6848,36 +6859,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="6.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.26171875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="24.26171875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="34" t="s">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="3" t="s">
         <v>75</v>
       </c>
@@ -6900,7 +6911,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="4" t="s">
         <v>77</v>
       </c>
@@ -6920,10 +6931,10 @@
         <v>183</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="4" t="s">
         <v>79</v>
       </c>
@@ -6943,10 +6954,10 @@
         <v>183</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="4" t="s">
         <v>81</v>
       </c>
@@ -6966,10 +6977,10 @@
         <v>183</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="4" t="s">
         <v>150</v>
       </c>
@@ -6989,10 +7000,10 @@
         <v>183</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="4" t="s">
         <v>85</v>
       </c>
@@ -7012,10 +7023,10 @@
         <v>183</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="4" t="s">
         <v>86</v>
       </c>
@@ -7035,10 +7046,10 @@
         <v>183</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="4" t="s">
         <v>95</v>
       </c>
@@ -7058,10 +7069,10 @@
         <v>183</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="4" t="s">
         <v>96</v>
       </c>
@@ -7081,10 +7092,10 @@
         <v>183</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="4" t="s">
         <v>122</v>
       </c>
@@ -7104,10 +7115,10 @@
         <v>183</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="4" t="s">
         <v>123</v>
       </c>
@@ -7127,10 +7138,10 @@
         <v>183</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="4" t="s">
         <v>124</v>
       </c>
@@ -7150,10 +7161,10 @@
         <v>183</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="4" t="s">
         <v>125</v>
       </c>
@@ -7173,55 +7184,55 @@
         <v>183</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="4" t="s">
         <v>195</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="14"/>
       <c r="E17" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="F17" s="18" t="s">
         <v>202</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>203</v>
       </c>
       <c r="G17" s="18"/>
       <c r="H17" s="18" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="34" t="s">
-        <v>196</v>
-      </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" s="43" t="s">
+        <v>269</v>
+      </c>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="3"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
       <c r="E21" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="H21" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="F21" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="H21" s="16" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="3" t="s">
         <v>75</v>
       </c>
@@ -7244,7 +7255,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="4" t="s">
         <v>195</v>
       </c>
@@ -7271,34 +7282,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.15625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="58" t="s">
         <v>90</v>
       </c>
       <c r="C3" s="58"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="13" t="s">
         <v>91</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="13" t="s">
         <v>92</v>
       </c>

</xml_diff>